<commit_message>
major updates to codebase
</commit_message>
<xml_diff>
--- a/instance_generator/generator_parameters.xlsx
+++ b/instance_generator/generator_parameters.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C4BF40-A313-47D3-B1F7-7D6C75DD344F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D8ED24-030E-4E8A-8D44-1D3BE3174E11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>base_node_id</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>number_of_vehicles</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,7 +407,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -428,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,7 +447,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -460,7 +463,15 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>